<commit_message>
thống kê phase 2
</commit_message>
<xml_diff>
--- a/docs/ack_statsitic.xlsx
+++ b/docs/ack_statsitic.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thuong\Documents\GitHub\Machine-Learning-Yearning-Vietnamese-Translation\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YourProjects\Machine-Learning-Yearning-Vietnamese-Translation\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7BF503-978D-4BEC-977A-43ABBAD1F7DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="15210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="15210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Phase 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>ngcthuong</t>
   </si>
@@ -133,11 +135,23 @@
   <si>
     <t>honghanhh</t>
   </si>
+  <si>
+    <t>rootonchair</t>
+  </si>
+  <si>
+    <t>Revise</t>
+  </si>
+  <si>
+    <t>Phản biện</t>
+  </si>
+  <si>
+    <t>samthehai</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -293,7 +307,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$4:$C$23</c:f>
+              <c:f>'Phase 1'!$C$4:$C$23</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -361,7 +375,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$23</c:f>
+              <c:f>'Phase 1'!$D$4:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -565,7 +579,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -573,6 +586,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -711,7 +725,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$29:$C$53</c:f>
+              <c:f>'Phase 1'!$C$29:$C$53</c:f>
               <c:strCache>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
@@ -794,7 +808,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$29:$D$53</c:f>
+              <c:f>'Phase 1'!$D$29:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1013,7 +1027,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1021,6 +1034,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1053,6 +1067,1308 @@
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Đóng</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> góp dịch bản hiệu đính</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.8573462049062991E-2"/>
+          <c:y val="0.10805458701826494"/>
+          <c:w val="0.90305128425951353"/>
+          <c:h val="0.65393923999969217"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Phase 2'!$A$1:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>nmdang</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ngcthuong</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>lkhphuc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>rootonchair</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tiepvupsu</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ngdthanhcs</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>thhung</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>khoapip</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>duythanhvn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Phase 2'!$B$1:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-05C8-436C-9360-37489263F1C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="586365808"/>
+        <c:axId val="534763600"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="586365808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="534763600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="534763600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="586365808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1"/>
+              <a:t>Đóng</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
+              <a:t> góp phản biện bản hiệu đính </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.27112800428346345"/>
+          <c:y val="5.0284445244016283E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Phase 2'!$A$13:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tiepvupsu</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ngcthuong</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>lkhphuc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>samthehai</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>rootonchair</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>quangnhat185</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sonvx</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>william-vu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Phase 2'!$B$13:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7623-4016-991B-CBF062923C96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="620717232"/>
+        <c:axId val="376363472"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="620717232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="376363472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="376363472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620717232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Đóng</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> góp bản hiệu đính</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Phase 2'!$A$1:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>nmdang</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ngcthuong</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>lkhphuc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>rootonchair</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tiepvupsu</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ngdthanhcs</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>thhung</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>khoapip</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>duythanhvn</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Phase 2'!$B$1:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F966-4FE6-9D8C-B5E2ED746915}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.75074540682414703"/>
+          <c:y val="0.2201363371245261"/>
+          <c:w val="0.23258792650918636"/>
+          <c:h val="0.70312992125984253"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1136,6 +2452,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2138,6 +3574,1595 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2443,6 +5468,119 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>298636</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>30256</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>598839</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6FCFA10-3A36-40F0-B456-EE49825AAE5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>296953</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>174809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>123264</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F714142C-2501-4FF2-8071-6CFA73CE2BE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>481853</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>135590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>168087</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D49668C1-9475-42FC-ADB4-9B50D0968ADF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2739,11 +5877,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3155,4 +6293,173 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B3AC81-7235-4287-BD56-E894AD88FEDF}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35:N36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A13:B21">
+    <sortCondition descending="1" ref="B14"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>